<commit_message>
New versions with swiss SAM
</commit_message>
<xml_diff>
--- a/03_7sec_sigAge/ALCONSC.xlsx
+++ b/03_7sec_sigAge/ALCONSC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5649873-4B52-4166-A74B-4954C7CC21F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0FF980-3FC8-4907-ADE4-8AF7F6686CA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>g1</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>s7</t>
+  </si>
+  <si>
+    <t>g4</t>
   </si>
 </sst>
 </file>
@@ -97,7 +100,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -384,15 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +425,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -414,10 +440,13 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -428,10 +457,13 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -442,10 +474,13 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -458,8 +493,11 @@
       <c r="D5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -470,10 +508,13 @@
         <v>10</v>
       </c>
       <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -484,10 +525,13 @@
         <v>20</v>
       </c>
       <c r="D7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -498,10 +542,13 @@
         <v>15</v>
       </c>
       <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B9">
         <f>SUM(B2:B8)</f>
         <v>100</v>
@@ -511,12 +558,26 @@
         <v>100</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D9" si="1">SUM(D2:D8)</f>
         <v>100</v>
       </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="2">SUM(E2:E8)</f>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B9:D9">
+  <conditionalFormatting sqref="B9:C9">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>100</formula>
     </cfRule>

</xml_diff>